<commit_message>
Last edits before presentation
</commit_message>
<xml_diff>
--- a/Project/match-reports/server/Template.xlsx
+++ b/Project/match-reports/server/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/855f74b0a7130c00/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/855f74b0a7130c00/Desktop/Coding/SportsScience/SportsScienceFall25/Project/match-reports/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="11_F25DC773A252ABDACC10480291DF7E465BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68A7197D-7505-41D6-8CFA-5CC58326A2BD}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="11_F25DC773A252ABDACC10480291DF7E465BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A143FD48-8B45-48E8-8D56-EFE6A875DADA}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="338" yWindow="1402" windowWidth="14400" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="2">
+  <futureMetadata name="XLRICHVALUE" count="1">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -37,27 +37,17 @@
         </ext>
       </extLst>
     </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="1"/>
-        </ext>
-      </extLst>
-    </bk>
   </futureMetadata>
-  <valueMetadata count="2">
+  <valueMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
-    <bk>
-      <rc t="1" v="1"/>
-    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Date:</t>
   </si>
@@ -68,10 +58,13 @@
     <t>SCU Soccer Weekly Load Report</t>
   </si>
   <si>
-    <t>Remarkably Low</t>
+    <t>Remarkably</t>
   </si>
   <si>
-    <t>Remarkably High</t>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
 </sst>
 </file>
@@ -101,7 +94,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +110,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA7A7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0504D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -133,27 +156,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -164,8 +193,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF4472C4"/>
+      <color rgb="FFC0504D"/>
+      <color rgb="FF991135"/>
+      <color rgb="FFFFA7A7"/>
       <color rgb="FFD9D9D9"/>
-      <color rgb="FF991135"/>
     </mruColors>
   </colors>
   <extLst>
@@ -224,37 +256,26 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
   <rv s="0">
     <v>0</v>
     <v>5</v>
   </rv>
-  <rv s="1">
-    <v>1</v>
-    <v>5</v>
-    <v>Blue and Red Gradient Lines" Poster for ...</v>
-  </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
   <s t="_localImage">
     <k n="_rvRel:LocalImageIdentifier" t="i"/>
     <k n="CalcOrigin" t="i"/>
   </s>
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-    <k n="Text" t="s"/>
-  </s>
 </rvStructures>
 </file>
 
 <file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
 <richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rel r:id="rId1"/>
-  <rel r:id="rId2"/>
 </richValueRels>
 </file>
 
@@ -521,23 +542,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="6.6640625" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" customWidth="1"/>
+    <col min="2" max="2" width="4.59765625" customWidth="1"/>
+    <col min="3" max="12" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="e" vm="1">
+      <c r="A1" s="11" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="11"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -546,30 +568,30 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="4" t="e" vm="1">
+      <c r="K1" s="11" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="L1" s="4"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -578,45 +600,47 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="7" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="2" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" s="7"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A5" s="2"/>
+      <c r="A5" s="10" t="s">
+        <v>1</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="8"/>
+      <c r="E5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
@@ -633,13 +657,24 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="2">
+    <mergeCell ref="K1:L3"/>
     <mergeCell ref="A1:B3"/>
-    <mergeCell ref="K1:L3"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>